<commit_message>
Finish inserting the data with pandas (Still need to arrange a pull of information)
</commit_message>
<xml_diff>
--- a/employeesystem/employeesystem/program/reports.xlsx
+++ b/employeesystem/employeesystem/program/reports.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>day</t>
   </si>
@@ -61,7 +61,7 @@
     <t>sum</t>
   </si>
   <si>
-    <t>vecation_day</t>
+    <t>vacation_day</t>
   </si>
   <si>
     <t>year</t>
@@ -79,13 +79,7 @@
     <t>Dor</t>
   </si>
   <si>
-    <t>eli</t>
-  </si>
-  <si>
     <t>zrihen</t>
-  </si>
-  <si>
-    <t>cohen</t>
   </si>
   <si>
     <t>benni</t>
@@ -531,16 +525,16 @@
         <v>55555</v>
       </c>
       <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
         <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
       </c>
       <c r="L2">
         <v>12</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Q2">
         <v>2020</v>
@@ -569,7 +563,7 @@
         <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K3">
         <v>656565</v>
@@ -604,7 +598,7 @@
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K4">
         <v>656565</v>
@@ -639,7 +633,7 @@
         <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K5">
         <v>656565</v>
@@ -653,34 +647,16 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>50</v>
-      </c>
-      <c r="E6">
-        <v>14</v>
-      </c>
-      <c r="F6">
-        <v>41</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H6">
         <v>6060</v>
       </c>
-      <c r="I6" t="s">
-        <v>23</v>
-      </c>
       <c r="L6">
         <v>7</v>
       </c>
-      <c r="O6">
-        <v>6.85</v>
+      <c r="P6">
+        <v>1</v>
       </c>
       <c r="Q6">
         <v>2020</v>

</xml_diff>